<commit_message>
Shacl file CV and Bodies
</commit_message>
<xml_diff>
--- a/05-Dataset5_org-ap-ep/04-SHACL/Dataset5_Bodies-Shapes.xlsx
+++ b/05-Dataset5_org-ap-ep/04-SHACL/Dataset5_Bodies-Shapes.xlsx
@@ -4,23 +4,18 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16385" windowHeight="8190" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16385" windowHeight="8190" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="class-based shapes" sheetId="1" r:id="rId1"/>
     <sheet name="class-based constraints" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="145621" iterateDelta="1E-4"/>
-  <extLst>
-    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="ExcelA1"/>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="121">
   <si>
     <t>Shapes URI</t>
   </si>
@@ -344,6 +339,49 @@
   </si>
   <si>
     <t>(skos:Concept org-ep:org-type)</t>
+  </si>
+  <si>
+    <t>ep-aut</t>
+  </si>
+  <si>
+    <t>http://data.europarl.europa.eu/authority/</t>
+  </si>
+  <si>
+    <t>dc:identifier</t>
+  </si>
+  <si>
+    <t>identifier</t>
+  </si>
+  <si>
+    <t>org-ep:hasCorporateBody</t>
+  </si>
+  <si>
+    <t>dc</t>
+  </si>
+  <si>
+    <t>http://purl.org/dc/elements/1.1/</t>
+  </si>
+  <si>
+    <t>An organisation has a Corporate Body.</t>
+  </si>
+  <si>
+    <t>hasCorporateBody</t>
+  </si>
+  <si>
+    <t>hasOrganizationType</t>
+  </si>
+  <si>
+    <t>^http://data.europarl.europa.eu/authority/notation-type/codict/.*$</t>
+  </si>
+  <si>
+    <t>^http://data.europarl.europa.eu/authority/committee-body/.*$
+^http://data.europarl.europa.eu/authority/delegation-body/.*$
+^http://data.europarl.europa.eu/authority/institution-body/.*$
+^http://data.europarl.europa.eu/authority/political-group-body/.*$
+^http://data.europarl.europa.eu/authority/governance-body/.*$</t>
+  </si>
+  <si>
+    <t>http://data.europarl.europa.eu/shapes/</t>
   </si>
 </sst>
 </file>
@@ -449,7 +487,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -500,6 +538,10 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
@@ -872,8 +914,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K23"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.54296875" defaultRowHeight="12.5" x14ac:dyDescent="0.5"/>
@@ -895,8 +937,8 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
+      <c r="B1" s="21" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.5">
@@ -1165,12 +1207,12 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T23"/>
+  <dimension ref="A1:T26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="8" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="9" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="P1" sqref="P1"/>
-      <selection pane="bottomLeft" activeCell="Q23" sqref="Q23"/>
+      <selection pane="bottomLeft" activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6796875" defaultRowHeight="12.5" x14ac:dyDescent="0.5"/>
@@ -1179,7 +1221,7 @@
     <col min="2" max="2" width="37" customWidth="1"/>
     <col min="3" max="3" width="40.40625" style="1" customWidth="1"/>
     <col min="4" max="4" width="15.54296875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="15.54296875" customWidth="1"/>
+    <col min="5" max="5" width="18.04296875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="29.26953125" style="1" customWidth="1"/>
     <col min="7" max="7" width="37" style="1" customWidth="1"/>
     <col min="8" max="8" width="25.40625" customWidth="1"/>
@@ -1229,212 +1271,204 @@
       <c r="D3" s="2"/>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.5">
-      <c r="C4" s="4"/>
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>108</v>
+      </c>
+      <c r="C4" s="22" t="s">
+        <v>109</v>
+      </c>
       <c r="D4" s="4"/>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.5">
-      <c r="A5" s="5" t="s">
+      <c r="A5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
+        <v>113</v>
+      </c>
+      <c r="C5" s="22" t="s">
+        <v>114</v>
+      </c>
+      <c r="D5" s="4"/>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.5">
+      <c r="A6" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="B5" s="6"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6"/>
-      <c r="H5" s="6"/>
-      <c r="I5" s="6"/>
-      <c r="J5" s="6"/>
-      <c r="K5" s="6"/>
-      <c r="L5" s="6"/>
-      <c r="M5" s="6"/>
-      <c r="N5" s="6"/>
-      <c r="O5" s="6"/>
-      <c r="P5" s="6"/>
-      <c r="Q5" s="6"/>
-      <c r="R5" s="8"/>
-      <c r="S5" s="8"/>
-      <c r="T5" s="8"/>
-    </row>
-    <row r="6" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="E6" s="1"/>
-      <c r="G6" s="4"/>
-      <c r="R6" s="1"/>
-    </row>
-    <row r="7" spans="1:20" s="11" customFormat="1" ht="73.45" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A7" s="11" t="s">
+      <c r="B6" s="6"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6"/>
+      <c r="J6" s="6"/>
+      <c r="K6" s="6"/>
+      <c r="L6" s="6"/>
+      <c r="M6" s="6"/>
+      <c r="N6" s="6"/>
+      <c r="O6" s="6"/>
+      <c r="P6" s="6"/>
+      <c r="Q6" s="6"/>
+      <c r="R6" s="8"/>
+      <c r="S6" s="8"/>
+      <c r="T6" s="8"/>
+    </row>
+    <row r="7" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="E7" s="1"/>
+      <c r="G7" s="4"/>
+      <c r="R7" s="1"/>
+    </row>
+    <row r="8" spans="1:20" s="11" customFormat="1" ht="73.45" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A8" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="B7" s="11" t="s">
+      <c r="B8" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="C8" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="D7" s="11" t="s">
+      <c r="D8" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="E7" s="11" t="s">
+      <c r="E8" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="F7" s="11" t="s">
+      <c r="F8" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="G7" s="11" t="s">
+      <c r="G8" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="H7" s="11" t="s">
+      <c r="H8" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="I7" s="11" t="s">
+      <c r="I8" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="J7" s="11" t="s">
+      <c r="J8" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="K7" s="11" t="s">
+      <c r="K8" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="L7" s="11" t="s">
+      <c r="L8" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="M7" s="11" t="s">
+      <c r="M8" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="N7" s="11" t="s">
+      <c r="N8" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="O7" s="11" t="s">
+      <c r="O8" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="P7" s="11" t="s">
+      <c r="P8" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="Q7" s="11" t="s">
+      <c r="Q8" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="R7" s="11" t="s">
+      <c r="R8" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="S7" s="11" t="s">
+      <c r="S8" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="T7" s="11" t="s">
+      <c r="T8" s="11" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="8" spans="1:20" ht="25" x14ac:dyDescent="0.5">
-      <c r="A8" s="16" t="s">
+    <row r="9" spans="1:20" ht="25" x14ac:dyDescent="0.5">
+      <c r="A9" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="16" t="s">
+      <c r="B9" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="C8" s="17" t="s">
+      <c r="C9" s="17" t="s">
         <v>65</v>
       </c>
-      <c r="D8" s="17" t="s">
+      <c r="D9" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="E8" s="18" t="s">
+      <c r="E9" s="18" t="s">
         <v>66</v>
       </c>
-      <c r="F8" s="16" t="s">
+      <c r="F9" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="G8" s="17" t="s">
+      <c r="G9" s="17" t="s">
         <v>68</v>
       </c>
-      <c r="H8" s="17" t="s">
+      <c r="H9" s="17" t="s">
         <v>69</v>
       </c>
-      <c r="I8" s="12" t="s">
+      <c r="I9" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="J8" s="12" t="s">
+      <c r="J9" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="K8" s="12" t="s">
+      <c r="K9" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="L8" s="17" t="s">
+      <c r="L9" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="M8" s="17" t="s">
+      <c r="M9" s="17" t="s">
         <v>73</v>
       </c>
-      <c r="N8" s="17" t="s">
+      <c r="N9" s="17" t="s">
         <v>74</v>
       </c>
-      <c r="O8" s="17" t="s">
+      <c r="O9" s="17" t="s">
         <v>75</v>
       </c>
-      <c r="P8" s="17" t="s">
+      <c r="P9" s="17" t="s">
         <v>76</v>
       </c>
-      <c r="Q8" s="17" t="s">
+      <c r="Q9" s="17" t="s">
         <v>77</v>
       </c>
-      <c r="R8" s="12" t="s">
+      <c r="R9" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="S8" s="17" t="s">
+      <c r="S9" s="17" t="s">
         <v>78</v>
       </c>
-      <c r="T8" s="17" t="s">
+      <c r="T9" s="17" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="9" spans="1:20" s="19" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A9" s="19" t="s">
+    <row r="10" spans="1:20" s="19" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A10" s="19" t="s">
         <v>80</v>
       </c>
-      <c r="T9" s="20"/>
-    </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.5">
-      <c r="A10" t="str">
-        <f t="shared" ref="A10:A16" si="0">CONCATENATE("epsh:P",ROW(A10))</f>
-        <v>epsh:P10</v>
-      </c>
-      <c r="B10" t="s">
-        <v>81</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D10" s="1">
-        <v>1</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="G10" s="1">
-        <v>1</v>
-      </c>
-      <c r="H10">
-        <v>1</v>
-      </c>
-      <c r="L10" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q10" s="1"/>
+      <c r="T10" s="20"/>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.5">
       <c r="A11" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="A11:A19" si="0">CONCATENATE("epsh:P",ROW(A11))</f>
         <v>epsh:P11</v>
       </c>
       <c r="B11" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>30</v>
       </c>
       <c r="D11" s="1">
-        <v>2</v>
-      </c>
-      <c r="E11" t="s">
-        <v>84</v>
+        <v>1</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>82</v>
       </c>
       <c r="G11" s="1">
         <v>1</v>
@@ -1443,28 +1477,26 @@
         <v>1</v>
       </c>
       <c r="L11" t="s">
-        <v>85</v>
-      </c>
-      <c r="M11" t="s">
-        <v>86</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="Q11" s="1"/>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.5">
       <c r="A12" t="str">
         <f t="shared" si="0"/>
         <v>epsh:P12</v>
       </c>
-      <c r="B12" s="3" t="s">
-        <v>87</v>
+      <c r="B12" t="s">
+        <v>83</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>30</v>
       </c>
       <c r="D12" s="1">
-        <v>3</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>88</v>
+        <v>2</v>
+      </c>
+      <c r="E12" t="s">
+        <v>84</v>
       </c>
       <c r="G12" s="1">
         <v>1</v>
@@ -1472,13 +1504,15 @@
       <c r="H12">
         <v>1</v>
       </c>
-      <c r="L12" s="3" t="s">
+      <c r="L12" t="s">
         <v>85</v>
       </c>
       <c r="M12" t="s">
-        <v>89</v>
-      </c>
-      <c r="R12" s="14"/>
+        <v>97</v>
+      </c>
+      <c r="R12" s="22" t="s">
+        <v>118</v>
+      </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.5">
       <c r="A13" t="str">
@@ -1486,16 +1520,16 @@
         <v>epsh:P13</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>30</v>
       </c>
       <c r="D13" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="G13" s="1">
         <v>1</v>
@@ -1503,48 +1537,42 @@
       <c r="H13">
         <v>1</v>
       </c>
-      <c r="L13" t="s">
+      <c r="L13" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="M13" s="3" t="s">
+      <c r="M13" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="14" spans="1:20" ht="50" x14ac:dyDescent="0.5">
+      <c r="R13" s="14"/>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.5">
       <c r="A14" t="str">
         <f t="shared" si="0"/>
         <v>epsh:P14</v>
       </c>
-      <c r="B14" t="s">
-        <v>92</v>
+      <c r="B14" s="3" t="s">
+        <v>90</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>30</v>
       </c>
       <c r="D14" s="1">
-        <v>5</v>
-      </c>
-      <c r="E14" t="s">
-        <v>93</v>
+        <v>4</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>91</v>
       </c>
       <c r="G14" s="1">
-        <v>24</v>
+        <v>1</v>
       </c>
       <c r="H14">
-        <v>24</v>
-      </c>
-      <c r="L14" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="L14" t="s">
         <v>85</v>
       </c>
       <c r="M14" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="R14" s="14"/>
-      <c r="S14" t="s">
-        <v>37</v>
-      </c>
-      <c r="T14" s="1" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
     </row>
     <row r="15" spans="1:20" ht="50" x14ac:dyDescent="0.5">
@@ -1552,17 +1580,17 @@
         <f t="shared" si="0"/>
         <v>epsh:P15</v>
       </c>
-      <c r="B15" s="3" t="s">
-        <v>95</v>
+      <c r="B15" t="s">
+        <v>92</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>30</v>
       </c>
       <c r="D15" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E15" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="G15" s="1">
         <v>24</v>
@@ -1576,182 +1604,292 @@
       <c r="M15" s="3" t="s">
         <v>94</v>
       </c>
+      <c r="R15" s="14"/>
+      <c r="S15" t="s">
+        <v>37</v>
+      </c>
       <c r="T15" s="1" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.5">
-      <c r="A16" s="3" t="str">
+    <row r="16" spans="1:20" ht="50" x14ac:dyDescent="0.5">
+      <c r="A16" t="str">
         <f t="shared" si="0"/>
         <v>epsh:P16</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>106</v>
+        <v>95</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>30</v>
       </c>
       <c r="D16" s="1">
+        <v>6</v>
+      </c>
+      <c r="E16" t="s">
+        <v>96</v>
+      </c>
+      <c r="G16" s="1">
+        <v>24</v>
+      </c>
+      <c r="H16">
+        <v>24</v>
+      </c>
+      <c r="L16" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="M16" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="T16" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.5">
+      <c r="A17" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>epsh:P17</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D17" s="1">
         <v>7</v>
       </c>
-      <c r="G16" s="1">
-        <v>1</v>
-      </c>
-      <c r="H16">
-        <v>1</v>
-      </c>
-      <c r="L16" t="s">
+      <c r="E17" t="s">
+        <v>117</v>
+      </c>
+      <c r="G17" s="1">
+        <v>1</v>
+      </c>
+      <c r="H17">
+        <v>1</v>
+      </c>
+      <c r="L17" t="s">
         <v>35</v>
       </c>
-      <c r="M16" t="s">
+      <c r="M17" t="s">
         <v>97</v>
       </c>
-      <c r="R16" s="14" t="s">
+      <c r="R17" s="14" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.5">
-      <c r="R17" s="14"/>
-    </row>
-    <row r="19" spans="1:20" s="19" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A19" s="19" t="s">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.5">
+      <c r="A18" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>epsh:P18</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D18" s="1">
+        <v>8</v>
+      </c>
+      <c r="E18" t="s">
+        <v>111</v>
+      </c>
+      <c r="G18" s="1">
+        <v>1</v>
+      </c>
+      <c r="H18">
+        <v>1</v>
+      </c>
+      <c r="L18" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="M18" t="s">
+        <v>86</v>
+      </c>
+      <c r="R18" s="14"/>
+    </row>
+    <row r="19" spans="1:20" ht="62.5" x14ac:dyDescent="0.5">
+      <c r="A19" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>epsh:P19</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D19" s="1">
+        <v>9</v>
+      </c>
+      <c r="E19" t="s">
+        <v>116</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="G19" s="1">
+        <v>1</v>
+      </c>
+      <c r="H19">
+        <v>1</v>
+      </c>
+      <c r="L19" t="s">
+        <v>35</v>
+      </c>
+      <c r="M19" t="s">
+        <v>97</v>
+      </c>
+      <c r="R19" s="23" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.5">
+      <c r="R20" s="14"/>
+    </row>
+    <row r="22" spans="1:20" s="19" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A22" s="19" t="s">
         <v>98</v>
       </c>
-      <c r="T19" s="20"/>
-    </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.5">
-      <c r="A20" t="str">
-        <f>CONCATENATE("epsh:P",ROW(A20))</f>
-        <v>epsh:P20</v>
-      </c>
-      <c r="B20" t="s">
-        <v>81</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D20" s="1">
-        <v>1</v>
-      </c>
-      <c r="E20" t="s">
-        <v>82</v>
-      </c>
-      <c r="G20" s="1">
-        <v>1</v>
-      </c>
-      <c r="H20">
-        <v>1</v>
-      </c>
-      <c r="J20" s="3"/>
-      <c r="L20" t="s">
-        <v>35</v>
-      </c>
-      <c r="R20" s="14"/>
-    </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.5">
-      <c r="A21" t="str">
-        <f>CONCATENATE("epsh:P",ROW(A21))</f>
-        <v>epsh:P21</v>
-      </c>
-      <c r="B21" t="s">
-        <v>83</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D21" s="1">
-        <v>2</v>
-      </c>
-      <c r="E21" t="s">
-        <v>84</v>
-      </c>
-      <c r="G21" s="1">
-        <v>1</v>
-      </c>
-      <c r="H21">
-        <v>1</v>
-      </c>
-      <c r="L21" t="s">
-        <v>85</v>
-      </c>
-      <c r="M21" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="22" spans="1:20" ht="50" x14ac:dyDescent="0.5">
-      <c r="A22" t="str">
-        <f>CONCATENATE("epsh:P",ROW(A22))</f>
-        <v>epsh:P22</v>
-      </c>
-      <c r="B22" t="s">
-        <v>99</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D22" s="1">
-        <v>3</v>
-      </c>
-      <c r="E22" t="s">
-        <v>93</v>
-      </c>
-      <c r="F22" s="15"/>
-      <c r="G22" s="1">
-        <v>24</v>
-      </c>
-      <c r="H22">
-        <v>24</v>
-      </c>
-      <c r="J22" s="3"/>
-      <c r="L22" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="M22" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="R22" s="14"/>
-      <c r="S22" t="s">
-        <v>37</v>
-      </c>
-      <c r="T22" s="1" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="23" spans="1:20" ht="37.5" x14ac:dyDescent="0.5">
+      <c r="T22" s="20"/>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.5">
       <c r="A23" t="str">
         <f>CONCATENATE("epsh:P",ROW(A23))</f>
         <v>epsh:P23</v>
       </c>
       <c r="B23" t="s">
-        <v>5</v>
+        <v>81</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>39</v>
       </c>
       <c r="D23" s="1">
+        <v>1</v>
+      </c>
+      <c r="E23" t="s">
+        <v>82</v>
+      </c>
+      <c r="G23" s="1">
+        <v>1</v>
+      </c>
+      <c r="H23">
+        <v>1</v>
+      </c>
+      <c r="J23" s="3"/>
+      <c r="L23" t="s">
+        <v>35</v>
+      </c>
+      <c r="R23" s="14"/>
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.5">
+      <c r="A24" t="str">
+        <f>CONCATENATE("epsh:P",ROW(A24))</f>
+        <v>epsh:P24</v>
+      </c>
+      <c r="B24" t="s">
+        <v>83</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D24" s="1">
+        <v>2</v>
+      </c>
+      <c r="E24" t="s">
+        <v>84</v>
+      </c>
+      <c r="G24" s="1">
+        <v>1</v>
+      </c>
+      <c r="H24">
+        <v>1</v>
+      </c>
+      <c r="L24" t="s">
+        <v>85</v>
+      </c>
+      <c r="M24" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="25" spans="1:20" ht="50" x14ac:dyDescent="0.5">
+      <c r="A25" t="str">
+        <f>CONCATENATE("epsh:P",ROW(A25))</f>
+        <v>epsh:P25</v>
+      </c>
+      <c r="B25" t="s">
+        <v>99</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D25" s="1">
+        <v>3</v>
+      </c>
+      <c r="E25" t="s">
+        <v>93</v>
+      </c>
+      <c r="F25" s="15"/>
+      <c r="G25" s="1">
+        <v>24</v>
+      </c>
+      <c r="H25">
+        <v>24</v>
+      </c>
+      <c r="J25" s="3"/>
+      <c r="L25" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="M25" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="R25" s="14"/>
+      <c r="S25" t="s">
+        <v>37</v>
+      </c>
+      <c r="T25" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="26" spans="1:20" ht="37.5" x14ac:dyDescent="0.5">
+      <c r="A26" t="str">
+        <f>CONCATENATE("epsh:P",ROW(A26))</f>
+        <v>epsh:P26</v>
+      </c>
+      <c r="B26" t="s">
+        <v>5</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D26" s="1">
         <v>4</v>
       </c>
-      <c r="E23" t="s">
+      <c r="E26" t="s">
         <v>101</v>
       </c>
-      <c r="F23" s="1" t="s">
+      <c r="F26" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="G23" s="1">
+      <c r="G26" s="1">
         <v>2</v>
       </c>
-      <c r="H23">
+      <c r="H26">
         <v>2</v>
       </c>
-      <c r="Q23" t="s">
+      <c r="Q26" t="s">
         <v>107</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B1" r:id="rId1"/>
-    <hyperlink ref="E8" r:id="rId2"/>
+    <hyperlink ref="E9" r:id="rId2"/>
     <hyperlink ref="C3" r:id="rId3"/>
+    <hyperlink ref="C4" r:id="rId4"/>
+    <hyperlink ref="R12" r:id="rId5" display="http://data.europarl.europa.eu/authority/notation-type/codict/.*$"/>
+    <hyperlink ref="R19" r:id="rId6" display="http://data.europarl.europa.eu/authority/delegation-body/.*$"/>
   </hyperlinks>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>